<commit_message>
Add API manual test cases
</commit_message>
<xml_diff>
--- a/art-gallery-tests.xlsx
+++ b/art-gallery-tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="132" windowWidth="11460" windowHeight="6912"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
   <si>
     <t>Project Name</t>
   </si>
@@ -294,6 +294,189 @@
   </si>
   <si>
     <t>Hien</t>
+  </si>
+  <si>
+    <t>API Testing</t>
+  </si>
+  <si>
+    <t>Get valid artwork by ID</t>
+  </si>
+  <si>
+    <t>Ensure API returns correct data when ID is valid</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/{id}</t>
+  </si>
+  <si>
+    <t>id = 22</t>
+  </si>
+  <si>
+    <t>200 OK, returns title, artist, image_id, etc.</t>
+  </si>
+  <si>
+    <t>Handle invalid artwork ID</t>
+  </si>
+  <si>
+    <t>Check API behavior when ID does not exist</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/999999</t>
+  </si>
+  <si>
+    <t>id = 999999</t>
+  </si>
+  <si>
+    <t>404 Not Found, with helpful error message</t>
+  </si>
+  <si>
+    <t>Handle negative ID</t>
+  </si>
+  <si>
+    <t>Confirm API rejects invalid negative input</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/-1</t>
+  </si>
+  <si>
+    <t>id = -1</t>
+  </si>
+  <si>
+    <t>Handle ID = 0</t>
+  </si>
+  <si>
+    <t>Check for proper response on edge case</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/0</t>
+  </si>
+  <si>
+    <t>id = 0</t>
+  </si>
+  <si>
+    <t>404 Not Found</t>
+  </si>
+  <si>
+    <t>Artwork with missing image_id</t>
+  </si>
+  <si>
+    <t>Ensure image_id can be missing and app handles it</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/45</t>
+  </si>
+  <si>
+    <t>id = 45</t>
+  </si>
+  <si>
+    <t>image_id = null, rest of data intact</t>
+  </si>
+  <si>
+    <t>Artwork with full image data</t>
+  </si>
+  <si>
+    <t>Check proper iiif_url and image_id are returned</t>
+  </si>
+  <si>
+    <t>Send GET request to /artworks/22</t>
+  </si>
+  <si>
+    <t>Valid image_id and iiif_url present</t>
+  </si>
+  <si>
+    <t>Response structure validity</t>
+  </si>
+  <si>
+    <t>Ensure response includes required fields</t>
+  </si>
+  <si>
+    <t>Send GET request to valid ID</t>
+  </si>
+  <si>
+    <t>Includes title, artist_title, image_id, etc.</t>
+  </si>
+  <si>
+    <t>API latency</t>
+  </si>
+  <si>
+    <t>Time how long the API takes to respond</t>
+  </si>
+  <si>
+    <t>Send GET request and measure response time</t>
+  </si>
+  <si>
+    <t>Response in &lt;500ms under normal conditions</t>
+  </si>
+  <si>
+    <t>API rate limiting</t>
+  </si>
+  <si>
+    <t>Check behavior when sending many requests quickly</t>
+  </si>
+  <si>
+    <t>Send many GET requests rapidly</t>
+  </si>
+  <si>
+    <t>IDs = 1 to 100 rapidly</t>
+  </si>
+  <si>
+    <t>Graceful rate limit or continues without crash</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>TC018</t>
+  </si>
+  <si>
+    <t>Public API is accessible</t>
+  </si>
+  <si>
+    <t>Public API is accessible, internet connected</t>
+  </si>
+  <si>
+    <t>200 OK, but empty data set</t>
+  </si>
+  <si>
+    <t>API returns 200 OK with empty data instead of 404</t>
+  </si>
+  <si>
+    <t>400 Bad Request</t>
+  </si>
+  <si>
+    <t>API rejects input with 400 Bad Request or similar error</t>
+  </si>
+  <si>
+    <t>200 OK,  returns the first page of artworks</t>
+  </si>
+  <si>
+    <t>API returned a list of artworks — not filtered by ID 0</t>
+  </si>
+  <si>
+    <t>Executed using Postman Collection Runner (manual batch test, not scripted automation).</t>
+  </si>
+  <si>
+    <t>No rate limiting observed up to 100 requests; API handles rapid calls gracefully.</t>
   </si>
 </sst>
 </file>
@@ -469,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -525,6 +708,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -543,8 +738,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,74 +1061,76 @@
     <col min="3" max="4" width="8.88671875" style="3"/>
     <col min="5" max="5" width="10.88671875" style="3" customWidth="1"/>
     <col min="6" max="6" width="18" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="8.88671875" style="22"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="22"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="26"/>
     </row>
     <row r="2" spans="1:17" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -1029,13 +1226,13 @@
       <c r="J6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="22" t="s">
         <v>49</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="19">
         <v>45846</v>
       </c>
       <c r="N6" s="2"/>
@@ -1043,7 +1240,7 @@
       <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1073,10 +1270,13 @@
       <c r="J7" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K7" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="19">
         <v>45846</v>
       </c>
       <c r="N7" s="2"/>
@@ -1084,7 +1284,7 @@
       <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1112,16 +1312,19 @@
       <c r="J8" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K8" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="19">
         <v>45846</v>
       </c>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1149,17 +1352,19 @@
       <c r="J9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="19">
         <v>45846</v>
       </c>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1189,17 +1394,19 @@
       <c r="J10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="19">
         <v>45846</v>
       </c>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1227,10 +1434,13 @@
       <c r="J11" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K11" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="19">
         <v>45847</v>
       </c>
     </row>
@@ -1265,11 +1475,13 @@
       <c r="J12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="19">
         <v>45847</v>
       </c>
       <c r="N12" s="4"/>
@@ -1305,10 +1517,13 @@
       <c r="J13" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="K13" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L13" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="19">
         <v>45847</v>
       </c>
     </row>
@@ -1343,20 +1558,391 @@
       <c r="J14" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="K14" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="L14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="19">
         <v>45847</v>
       </c>
     </row>
+    <row r="15" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="19">
+        <v>45853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="19">
+        <v>45854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M18" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M21" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M22" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="19">
+        <v>45855</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A15:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add 4 backend API test cases into manual testing document
</commit_message>
<xml_diff>
--- a/art-gallery-tests.xlsx
+++ b/art-gallery-tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="178">
   <si>
     <t>Project Name</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Hien</t>
   </si>
   <si>
-    <t>API Testing</t>
-  </si>
-  <si>
     <t>Get valid artwork by ID</t>
   </si>
   <si>
@@ -477,13 +474,220 @@
   </si>
   <si>
     <t>No rate limiting observed up to 100 requests; API handles rapid calls gracefully.</t>
+  </si>
+  <si>
+    <t>Backend API Testing</t>
+  </si>
+  <si>
+    <t>Get First Artwork</t>
+  </si>
+  <si>
+    <t>Verify that the first artwork is returned successfully</t>
+  </si>
+  <si>
+    <t>Backend is running</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Send GET request to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/api/artwork</t>
+    </r>
+  </si>
+  <si>
+    <t>Get Next Artwork</t>
+  </si>
+  <si>
+    <t>Verify that the next artwork is returned</t>
+  </si>
+  <si>
+    <t>Get Previous Artwork</t>
+  </si>
+  <si>
+    <t>Verify that the previous artwork is returned properly</t>
+  </si>
+  <si>
+    <t>Artwork has navigated forward</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Send GET to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/api/artwork/previous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Observe that artwork goes back one step</t>
+    </r>
+  </si>
+  <si>
+    <t>JSON Response Format</t>
+  </si>
+  <si>
+    <t>Validate structure of returned artwork object</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JSON includes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>artist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>imgUrl</t>
+    </r>
+  </si>
+  <si>
+    <t>Check for null/missing fields too</t>
+  </si>
+  <si>
+    <t>TC019</t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>TC021</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>Backend is running; Initial artwork loaded</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Send GET request to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/api/artwork/next
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Observe that artwork changes from previous</t>
+    </r>
+  </si>
+  <si>
+    <t>HTTP 200 OK;
+JSON includes artwork title, artist, and image URL</t>
+  </si>
+  <si>
+    <t>HTTP 200 OK;
+JSON with new artwork data different from previous</t>
+  </si>
+  <si>
+    <t>HTTP 200 OK;
+JSON with previous artwork data</t>
+  </si>
+  <si>
+    <t>External API Testing
+ (Art Institute of Chicago)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Send GET to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/api/artwork
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. Inspect JSON keys and value types</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +743,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -652,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -723,6 +933,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -737,9 +956,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,67 +1286,67 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:17" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="29"/>
     </row>
     <row r="3" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -1240,7 +1456,7 @@
       <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1284,7 +1500,7 @@
       <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1324,7 +1540,7 @@
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1364,7 +1580,7 @@
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1406,7 +1622,7 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1569,29 +1785,29 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="D15" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F15" s="20" t="s">
+      <c r="G15" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="H15" s="20" t="s">
         <v>96</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>97</v>
       </c>
       <c r="I15" s="21" t="s">
         <v>9</v>
@@ -1610,36 +1826,36 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="E16" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="H16" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>102</v>
-      </c>
       <c r="I16" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J16" s="20" t="s">
         <v>48</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>91</v>
@@ -1649,30 +1865,30 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="E17" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F17" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>106</v>
-      </c>
       <c r="H17" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J17" s="20" t="s">
         <v>10</v>
@@ -1688,36 +1904,36 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="E18" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F18" s="20" t="s">
+      <c r="G18" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="H18" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>111</v>
-      </c>
       <c r="I18" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J18" s="20" t="s">
         <v>48</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>91</v>
@@ -1727,27 +1943,27 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C19" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="E19" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="20" t="s">
+      <c r="G19" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>116</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>9</v>
@@ -1766,27 +1982,27 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="E20" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" s="20" t="s">
+      <c r="G20" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="I20" s="22" t="s">
         <v>9</v>
@@ -1805,27 +2021,27 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="E21" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F21" s="20" t="s">
+      <c r="G21" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>124</v>
       </c>
       <c r="I21" s="22" t="s">
         <v>9</v>
@@ -1844,27 +2060,27 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="E22" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="20" t="s">
+      <c r="G22" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>128</v>
       </c>
       <c r="I22" s="22" t="s">
         <v>9</v>
@@ -1883,36 +2099,36 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="F23" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F23" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="H23" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="20" t="s">
-        <v>133</v>
-      </c>
       <c r="I23" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J23" s="20" t="s">
         <v>10</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>91</v>
@@ -1921,28 +2137,173 @@
         <v>45855</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="29"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
+    <row r="24" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M24" s="24">
+        <v>45866</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M25" s="24">
+        <v>45866</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
+      <c r="B26" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" s="24">
+        <v>45866</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
+      <c r="B27" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="24">
+        <v>45866</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A24:A27"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>